<commit_message>
Reporte y cifras del 3 de Julio 2022
</commit_message>
<xml_diff>
--- a/2022/Reporte2022.xlsx
+++ b/2022/Reporte2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexPC\Documents\BotVialLogs\src\botvialcdmx\Logs de la aplicacion\2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexPC\Documents\Repositorio Github BotVialCDMX\BotVialCDMX\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426C3017-45BB-44E5-B426-86ACB53D2961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB96C537-340F-4FC4-9163-C926B42BF181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="601" activeTab="1" xr2:uid="{36ADE04C-9BFA-4982-BEF0-6418EFF0400B}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" tabRatio="601" activeTab="1" xr2:uid="{36ADE04C-9BFA-4982-BEF0-6418EFF0400B}"/>
   </bookViews>
   <sheets>
     <sheet name="Totales Junio" sheetId="2" r:id="rId1"/>
@@ -713,7 +713,7 @@
   <dimension ref="A2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -828,7 +828,33 @@
       <c r="A5" s="2">
         <v>44745</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="B5">
+        <v>78</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2">

</xml_diff>

<commit_message>
Actualización de logs y cifras del 4 de Julio 2022
</commit_message>
<xml_diff>
--- a/2022/Reporte2022.xlsx
+++ b/2022/Reporte2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexPC\Documents\Repositorio Github BotVialCDMX\BotVialCDMX\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB96C537-340F-4FC4-9163-C926B42BF181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB7FF67-B3EB-49F1-9122-66A0825B5DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" tabRatio="601" activeTab="1" xr2:uid="{36ADE04C-9BFA-4982-BEF0-6418EFF0400B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" activeTab="1" xr2:uid="{36ADE04C-9BFA-4982-BEF0-6418EFF0400B}"/>
   </bookViews>
   <sheets>
     <sheet name="Totales Junio" sheetId="2" r:id="rId1"/>
@@ -524,19 +524,19 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="20.453125" customWidth="1"/>
-    <col min="7" max="9" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="9" width="17.85546875" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44739</v>
       </c>
@@ -600,7 +600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44740</v>
       </c>
@@ -632,7 +632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44741</v>
       </c>
@@ -664,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44742</v>
       </c>
@@ -696,7 +696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I7" s="5"/>
     </row>
   </sheetData>
@@ -713,22 +713,22 @@
   <dimension ref="A2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="20.453125" customWidth="1"/>
-    <col min="7" max="9" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="9" width="17.85546875" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,7 +760,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44743</v>
       </c>
@@ -792,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44744</v>
       </c>
@@ -824,7 +824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44745</v>
       </c>
@@ -856,169 +856,195 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44746</v>
       </c>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>97</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44747</v>
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44748</v>
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44749</v>
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44750</v>
       </c>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44751</v>
       </c>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44752</v>
       </c>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44753</v>
       </c>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44754</v>
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44755</v>
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44756</v>
       </c>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44757</v>
       </c>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44758</v>
       </c>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44759</v>
       </c>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44760</v>
       </c>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44761</v>
       </c>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44762</v>
       </c>
       <c r="I22" s="4"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44763</v>
       </c>
       <c r="I23" s="4"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44764</v>
       </c>
       <c r="I24" s="4"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44765</v>
       </c>
       <c r="I25" s="4"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44766</v>
       </c>
       <c r="I26" s="4"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44767</v>
       </c>
       <c r="I27" s="4"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44768</v>
       </c>
       <c r="I28" s="4"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44769</v>
       </c>
       <c r="I29" s="4"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44770</v>
       </c>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44771</v>
       </c>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44772</v>
       </c>
       <c r="I32" s="4"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44773</v>
       </c>

</xml_diff>

<commit_message>
07-07-22 - Se actualizan cifras del 6 y 7 de Julio 2022
</commit_message>
<xml_diff>
--- a/2022/Reporte2022.xlsx
+++ b/2022/Reporte2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexPC\Documents\Repositorio Github BotVialCDMX\BotVialCDMX\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB7FF67-B3EB-49F1-9122-66A0825B5DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368D34F2-C09F-4D12-867E-82F381D3EBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" activeTab="1" xr2:uid="{36ADE04C-9BFA-4982-BEF0-6418EFF0400B}"/>
   </bookViews>
@@ -713,7 +713,7 @@
   <dimension ref="A2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,13 +892,65 @@
       <c r="A7" s="2">
         <v>44747</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="B7">
+        <v>78</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44748</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="B8">
+        <v>92</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -994,6 +1046,7 @@
       <c r="A24" s="2">
         <v>44764</v>
       </c>
+      <c r="F24" s="5"/>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cifras del 7 y 8 de Julio 2022
</commit_message>
<xml_diff>
--- a/2022/Reporte2022.xlsx
+++ b/2022/Reporte2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexPC\Documents\Repositorio Github BotVialCDMX\BotVialCDMX\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368D34F2-C09F-4D12-867E-82F381D3EBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB57805-2B90-4049-A64A-CC6010F27FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" activeTab="1" xr2:uid="{36ADE04C-9BFA-4982-BEF0-6418EFF0400B}"/>
   </bookViews>
@@ -521,7 +521,7 @@
   <dimension ref="A2:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +713,7 @@
   <dimension ref="A2:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,13 +956,65 @@
       <c r="A9" s="2">
         <v>44749</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="B9">
+        <v>91</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44750</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="B10">
+        <v>114</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">

</xml_diff>

<commit_message>
Se incorporan logs de Julio. Se actualizar README.md
</commit_message>
<xml_diff>
--- a/2022/Reporte2022.xlsx
+++ b/2022/Reporte2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexPC\Documents\Repositorio Github BotVialCDMX\BotVialCDMX\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB57805-2B90-4049-A64A-CC6010F27FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE45961F-CB83-4ECD-8539-9A88A4976A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" activeTab="1" xr2:uid="{36ADE04C-9BFA-4982-BEF0-6418EFF0400B}"/>
+    <workbookView xWindow="-23565" yWindow="0" windowWidth="21945" windowHeight="15540" tabRatio="601" activeTab="1" xr2:uid="{36ADE04C-9BFA-4982-BEF0-6418EFF0400B}"/>
   </bookViews>
   <sheets>
     <sheet name="Totales Junio" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Fecha</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Motociclista Fallecido</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -121,7 +124,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -195,7 +222,7 @@
     <tableColumn id="6" xr3:uid="{53D60708-8B5B-440D-9467-6C31CD30A8E6}" name="Ciclista Atropellado"/>
     <tableColumn id="7" xr3:uid="{E0109DE1-AB33-4C3C-B8FE-E66EF554ECA6}" name="Peaton Fallecido"/>
     <tableColumn id="8" xr3:uid="{879924B8-FCE4-4B2A-998F-5416D13A6FD5}" name="Ciclista Fallecido"/>
-    <tableColumn id="10" xr3:uid="{3DD72D2C-A3B0-4833-AFDC-6EFB9DA50319}" name="Motociclista Fallecido" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{3DD72D2C-A3B0-4833-AFDC-6EFB9DA50319}" name="Motociclista Fallecido" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{EA93CF98-CC33-4F21-AADD-26E064804565}" name="Automovilista Fallecido"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -203,19 +230,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{09B69712-BCAF-4ECD-A27D-D91879C365B0}" name="Tabla13" displayName="Tabla13" ref="A2:J33" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{09B69712-BCAF-4ECD-A27D-D91879C365B0}" name="Tabla13" displayName="Tabla13" ref="A2:J34" totalsRowCount="1">
   <autoFilter ref="A2:J33" xr:uid="{9B30534C-9291-458F-B76E-DC04609D31A7}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{972BD168-8644-48D1-92A6-D910CE0E6751}" name="Fecha"/>
+    <tableColumn id="1" xr3:uid="{972BD168-8644-48D1-92A6-D910CE0E6751}" name="Fecha" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{DC13F8AB-6118-4015-8E7B-30FF4CE4A6A9}" name="Total Eventos Identificados"/>
-    <tableColumn id="3" xr3:uid="{1DC6EEBC-7AA7-4036-A44A-4118DA13445A}" name="Volcaduras"/>
-    <tableColumn id="4" xr3:uid="{41A26E44-8517-4591-B5DC-77DAAF89636A}" name="Peaton Atropellado"/>
-    <tableColumn id="5" xr3:uid="{BFA984B8-BCF6-4A3B-8B7E-892FE016B1E4}" name="Motocilista Atropellado"/>
-    <tableColumn id="6" xr3:uid="{F7EE3DC7-7AC4-49F8-B300-4F7B0EB79AB6}" name="Ciclista Atropellado"/>
-    <tableColumn id="7" xr3:uid="{54498FF1-2992-444D-A6A0-9DF1EB93337C}" name="Peaton Fallecido"/>
-    <tableColumn id="8" xr3:uid="{4C5A860A-E7B8-464F-9548-4D30DBDA790B}" name="Ciclista Fallecido"/>
-    <tableColumn id="10" xr3:uid="{2C812E3B-2F27-4EA6-B74C-935E1EFC3817}" name="Motociclista Fallecido" dataDxfId="0"/>
-    <tableColumn id="9" xr3:uid="{5428AD79-C666-4058-AE4E-B8757DF63D96}" name="Automovilista Fallecido"/>
+    <tableColumn id="3" xr3:uid="{1DC6EEBC-7AA7-4036-A44A-4118DA13445A}" name="Volcaduras" totalsRowFunction="sum"/>
+    <tableColumn id="4" xr3:uid="{41A26E44-8517-4591-B5DC-77DAAF89636A}" name="Peaton Atropellado" totalsRowFunction="sum"/>
+    <tableColumn id="5" xr3:uid="{BFA984B8-BCF6-4A3B-8B7E-892FE016B1E4}" name="Motocilista Atropellado" totalsRowFunction="sum"/>
+    <tableColumn id="6" xr3:uid="{F7EE3DC7-7AC4-49F8-B300-4F7B0EB79AB6}" name="Ciclista Atropellado" totalsRowFunction="sum"/>
+    <tableColumn id="7" xr3:uid="{54498FF1-2992-444D-A6A0-9DF1EB93337C}" name="Peaton Fallecido" totalsRowFunction="sum"/>
+    <tableColumn id="8" xr3:uid="{4C5A860A-E7B8-464F-9548-4D30DBDA790B}" name="Ciclista Fallecido" totalsRowFunction="sum"/>
+    <tableColumn id="10" xr3:uid="{2C812E3B-2F27-4EA6-B74C-935E1EFC3817}" name="Motociclista Fallecido" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{5428AD79-C666-4058-AE4E-B8757DF63D96}" name="Automovilista Fallecido" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -710,10 +737,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E49774-4289-4AE6-8821-14C890E26857}">
-  <dimension ref="A2:J33"/>
+  <dimension ref="A2:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,140 +1047,558 @@
       <c r="A11" s="2">
         <v>44751</v>
       </c>
-      <c r="I11" s="4"/>
+      <c r="B11">
+        <v>81</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44752</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="B12">
+        <v>51</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44753</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="B13">
+        <v>73</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44754</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="B14">
+        <v>83</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44755</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="B15">
+        <v>87</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44756</v>
       </c>
-      <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>104</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44757</v>
       </c>
-      <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>78</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44758</v>
       </c>
-      <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>97</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" s="4">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44759</v>
       </c>
-      <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>75</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="4">
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44760</v>
       </c>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>96</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44761</v>
       </c>
-      <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>57</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44762</v>
       </c>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>73</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44763</v>
       </c>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>79</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44764</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>83</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44765</v>
       </c>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>46</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44766</v>
       </c>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44767</v>
       </c>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44768</v>
       </c>
-      <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44769</v>
       </c>
-      <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44770</v>
       </c>
-      <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44771</v>
       </c>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44772</v>
       </c>
-      <c r="I32" s="4"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44773</v>
       </c>
-      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <f>SUBTOTAL(109,Tabla13[Volcaduras])</f>
+        <v>91</v>
+      </c>
+      <c r="D34">
+        <f>SUBTOTAL(109,Tabla13[Peaton Atropellado])</f>
+        <v>53</v>
+      </c>
+      <c r="E34">
+        <f>SUBTOTAL(109,Tabla13[Motocilista Atropellado])</f>
+        <v>33</v>
+      </c>
+      <c r="F34">
+        <f>SUBTOTAL(109,Tabla13[Ciclista Atropellado])</f>
+        <v>5</v>
+      </c>
+      <c r="G34">
+        <f>SUBTOTAL(109,Tabla13[Peaton Fallecido])</f>
+        <v>8</v>
+      </c>
+      <c r="H34">
+        <f>SUBTOTAL(109,Tabla13[Ciclista Fallecido])</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="4">
+        <f>SUBTOTAL(109,Tabla13[Motociclista Fallecido])</f>
+        <v>16</v>
+      </c>
+      <c r="J34">
+        <f>SUBTOTAL(109,Tabla13[Automovilista Fallecido])</f>
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>